<commit_message>
UI Overhaul: Add Sidebar with Categories, Regenerate All Content
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,6 +441,16 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>banner_type</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>prompt</t>
         </is>
       </c>
@@ -453,7 +463,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>자세하고 유익한 블로그 포스팅을 작성해줘</t>
+          <t>AI 그림</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>tech</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Write a blog post about 미드저니 실사 고양이 프롬프트</t>
         </is>
       </c>
     </row>
@@ -465,7 +485,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>자세하고 유익한 블로그 포스팅을 작성해줘</t>
+          <t>유튜브</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>book</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Write a blog post about 유튜브 쇼츠 공포 썰 대본 예시</t>
         </is>
       </c>
     </row>
@@ -477,7 +507,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>자세하고 유익한 블로그 포스팅을 작성해줘</t>
+          <t>업무 효율</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>general</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Write a blog post about ChatGPT 영어 비즈니스 이메일 작성법</t>
         </is>
       </c>
     </row>
@@ -489,7 +529,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>자세하고 유익한 블로그 포스팅을 작성해줘</t>
+          <t>AI 그림</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>tech</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Write a blog post about 스테이블 디퓨전 3D 캐릭터 모델 추천</t>
         </is>
       </c>
     </row>
@@ -501,7 +551,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>자세하고 유익한 블로그 포스팅을 작성해줘</t>
+          <t>생산성</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>general</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Write a blog post about 노션으로 독서 기록 템플릿 만들기</t>
         </is>
       </c>
     </row>
@@ -513,7 +573,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>자세하고 유익한 블로그 포스팅을 작성해줘</t>
+          <t>디자인</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>tech</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Write a blog post about AI 로고 디자인 무료 사이트 추천</t>
         </is>
       </c>
     </row>
@@ -525,7 +595,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>자세하고 유익한 블로그 포스팅을 작성해줘</t>
+          <t>블로그</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>book</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Write a blog post about 블로그 글쓰기 자동화 프롬프트</t>
         </is>
       </c>
     </row>
@@ -537,7 +617,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>자세하고 유익한 블로그 포스팅을 작성해줘</t>
+          <t>SNS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>general</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Write a blog post about 인스타그램 감성 글귀 생성 프롬프트</t>
         </is>
       </c>
     </row>
@@ -549,7 +639,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>자세하고 유익한 블로그 포스팅을 작성해줘</t>
+          <t>코딩</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>tech</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Write a blog post about 파이썬 업무 자동화 코드 예시</t>
         </is>
       </c>
     </row>
@@ -561,7 +661,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>자세하고 유익한 블로그 포스팅을 작성해줘</t>
+          <t>마케팅</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>book</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Write a blog post about 스마트스토어 상세페이지 카피라이팅</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
UX Upgrade: Hero Search, SEO, and 20+ Categorized Posts
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,237 +441,352 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>prompt</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>category</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>banner_type</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>prompt</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>미드저니 실사 고양이 프롬프트</t>
+          <t>Instagram Viral Caption Generator</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>AI 그림</t>
+          <t>Write a viral caption for...</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>tech</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Write a blog post about 미드저니 실사 고양이 프롬프트</t>
+          <t>Marketing</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>유튜브 쇼츠 공포 썰 대본 예시</t>
+          <t>Python Code Debugger</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>유튜브</t>
+          <t>Write a viral caption for...</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>book</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Write a blog post about 유튜브 쇼츠 공포 썰 대본 예시</t>
+          <t>Coding</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ChatGPT 영어 비즈니스 이메일 작성법</t>
+          <t>SEO Blog Post Writer</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>업무 효율</t>
+          <t>Write a viral caption for...</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>general</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Write a blog post about ChatGPT 영어 비즈니스 이메일 작성법</t>
+          <t>Writing</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>스테이블 디퓨전 3D 캐릭터 모델 추천</t>
+          <t>Email Cold Outreach Template</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>AI 그림</t>
+          <t>Write a viral caption for...</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>tech</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Write a blog post about 스테이블 디퓨전 3D 캐릭터 모델 추천</t>
+          <t>Business</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>노션으로 독서 기록 템플릿 만들기</t>
+          <t>Midjourney Portrait Prompt</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>생산성</t>
+          <t>Write a viral caption for...</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>general</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Write a blog post about 노션으로 독서 기록 템플릿 만들기</t>
+          <t>Art</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AI 로고 디자인 무료 사이트 추천</t>
+          <t>YouTube Video Script Hook</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>디자인</t>
+          <t>Write a viral caption for...</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>tech</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Write a blog post about AI 로고 디자인 무료 사이트 추천</t>
+          <t>Marketing</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>블로그 글쓰기 자동화 프롬프트</t>
+          <t>React Component Generator</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>블로그</t>
+          <t>Write a viral caption for...</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>book</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Write a blog post about 블로그 글쓰기 자동화 프롬프트</t>
+          <t>Coding</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>인스타그램 감성 글귀 생성 프롬프트</t>
+          <t>Business Plan Executive Summary</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>SNS</t>
+          <t>Write a viral caption for...</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>general</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>Write a blog post about 인스타그램 감성 글귀 생성 프롬프트</t>
+          <t>Business</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>파이썬 업무 자동화 코드 예시</t>
+          <t>Fitness Workout Plan AI</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>코딩</t>
+          <t>Write a viral caption for...</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>tech</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Write a blog post about 파이썬 업무 자동화 코드 예시</t>
+          <t>Lifestyle</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>스마트스토어 상세페이지 카피라이팅</t>
+          <t>Meditation Script Generator</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>마케팅</t>
+          <t>Write a viral caption for...</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>book</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Write a blog post about 스마트스토어 상세페이지 카피라이팅</t>
+          <t>Lifestyle</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>TikTok Trend Ideas</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Write a viral caption for...</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SQL Query Optimizer</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Write a viral caption for...</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Coding</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Resume Bullet Point Polisher</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Write a viral caption for...</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Recipe Generator from Ingredients</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Write a viral caption for...</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Lifestyle</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Startup Pitch Deck Outliner</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Write a viral caption for...</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Business</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Twitter Thread Creator</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Write a viral caption for...</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Excel Formula Explainer</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Write a viral caption for...</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Coding</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Novel Character Backstory</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Write a viral caption for...</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Writing</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Product Description Improver</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Write a viral caption for...</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Marketing</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Daily Journaling Prompts</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Write a viral caption for...</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Lifestyle</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto-Deploy: New Content from Factory
</commit_message>
<xml_diff>
--- a/list.xlsx
+++ b/list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\visual\lazyprompt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D25A09-FCDB-495A-AA98-74BFB4D03F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7FF0AF-D6F7-4B4A-BE28-B1E90CD18F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="46">
   <si>
     <t>topic</t>
   </si>
@@ -31,136 +31,133 @@
     <t>category</t>
   </si>
   <si>
-    <t>인스타그램 바이럴 캡션 생성기</t>
-  </si>
-  <si>
-    <t>인스타그램 게시물에 사용할 바이럴하고 참여를 유도하는 매력적인 캡션을 작성해줘. 이모지를 적절히 사용하고, 독자에게 질문을 던져 댓글을 유도하는 마무리로 끝내줘.</t>
-  </si>
-  <si>
     <t>마케팅</t>
   </si>
   <si>
-    <t>파이썬 코드 디버거</t>
-  </si>
-  <si>
-    <t>내가 제공하는 파이썬 코드의 버그를 찾아서 수정하고, 왜 에러가 발생했는지 초보자도 이해하기 쉽게 설명해줘. 또한, 성능을 개선할 수 있는 팁도 함께 알려줘.</t>
-  </si>
-  <si>
     <t>코딩</t>
   </si>
   <si>
-    <t>SEO 블로그 포스팅 작성기</t>
-  </si>
-  <si>
-    <t>검색 엔진 최적화(SEO)를 고려하여 블로그 글을 작성해줘. 제목은 클릭을 유도하도록 짓고, 본문에는 관련 키워드를 자연스럽게 녹여내줘. 소제목을 사용하여 가독성을 높여줘.</t>
-  </si>
-  <si>
     <t>글쓰기</t>
   </si>
   <si>
-    <t>콜드 메일 영업 템플릿</t>
-  </si>
-  <si>
-    <t>잠재 고객에게 보낼 매력적인 콜드 메일(영업 메일) 템플릿을 작성해줘. 메일을 열어보게 만드는 제목과, 짧고 간결하면서도 신뢰를 주는 본문 내용으로 구성해줘.</t>
-  </si>
-  <si>
     <t>비즈니스</t>
   </si>
   <si>
-    <t>미드저니 인물화 프롬프트</t>
-  </si>
-  <si>
-    <t>미드저니(Midjourney) AI에서 고퀄리티 인물화를 생성하기 위한 프롬프트를 작성해줘. 조명, 화풍, 카메라 앵글, 묘사 세부 사항 등을 포함하여 영어 프롬프트로 만들어줘.</t>
-  </si>
-  <si>
-    <t>예술</t>
-  </si>
-  <si>
-    <t>유튜브 영상 도입부 대본</t>
-  </si>
-  <si>
-    <t>유튜브 영상의 초반 5초 안에 시청자를 사로잡을 수 있는 강력한 도입부(후킹) 대본을 3가지 버전으로 작성해줘. 호기심을 자극하거나 공감을 이끌어내는 멘트를 사용해줘.</t>
-  </si>
-  <si>
-    <t>리액트 컴포넌트 생성기</t>
-  </si>
-  <si>
-    <t>특정 기능을 수행하는 리액트(React) 컴포넌트 코드를 작성해줘. 함수형 컴포넌트로 작성하고, 스타일링을 위한 CSS나 Tailwind 클래스 예시도 포함해줘. 주석으로 설명을 달아줘.</t>
-  </si>
-  <si>
-    <t>사업계획서 요약본 작성</t>
-  </si>
-  <si>
-    <t>투자자에게 보여줄 사업계획서의 요약본(Executive Summary)을 작성해줘. 문제 제기, 해결책, 시장 규모, 비즈니스 모델, 경쟁 우위를 명확하고 설득력 있게 정리해줘.</t>
-  </si>
-  <si>
-    <t>AI 피트니스 운동 계획표</t>
-  </si>
-  <si>
-    <t>사용자의 목표(예: 다이어트, 근육 증가)와 운동 수준에 맞춘 일주일치 운동 루틴을 표로 작성해줘. 각 요일별 운동 종목, 세트 수, 횟수, 휴식 시간을 구체적으로 알려줘.</t>
-  </si>
-  <si>
-    <t>라이프스타일</t>
-  </si>
-  <si>
-    <t>명상 스크립트 생성기</t>
-  </si>
-  <si>
-    <t>10분 동안 편안하게 들을 수 있는 명상 가이드 스크립트를 작성해줘. 호흡에 집중하고 몸의 긴장을 푸는 내용을 포함하여, 차분하고 부드러운 어조로 써줘.</t>
-  </si>
-  <si>
-    <t>틱톡 숏폼 트렌드 아이디어</t>
-  </si>
-  <si>
-    <t>현재 틱톡이나 릴스에서 유행할 만한 숏폼 콘텐츠 아이디어를 5가지만 제안해줘. 각 아이디어별로 촬영 컨셉, 사용하는 음악 스타일, 기대 효과를 설명해줘.</t>
-  </si>
-  <si>
-    <t>SQL 쿼리 최적화</t>
-  </si>
-  <si>
-    <t>복잡하고 느린 SQL 쿼리를 더 효율적으로 동작하도록 최적화해줘. 쿼리의 성능을 개선하는 방법과 인덱스 활용 팁을 함께 설명해줘.</t>
-  </si>
-  <si>
-    <t>이력서 성과 요약 다듬기</t>
-  </si>
-  <si>
-    <t>이력서에 들어갈 경력 기술서의 불렛 포인트(Bullet points)를 더 전문적이고 성과 중심적으로 다듬어줘. 수치(%)나 구체적인 결과를 포함하여 임팩트 있게 바꿔줘.</t>
-  </si>
-  <si>
-    <t>냉장고 재료 레시피 생성</t>
-  </si>
-  <si>
-    <t>현재 냉장고에 있는 재료들을 입력하면, 만들 수 있는 맛있는 요리 레시피 3가지를 추천해줘. 조리 방법과 예상 소요 시간, 난이도를 함께 알려줘.</t>
-  </si>
-  <si>
-    <t>스타트업 피치덱 개요</t>
-  </si>
-  <si>
-    <t>초기 스타트업이 투자 유치를 위해 사용할 피치덱(발표 자료)의 슬라이드별 목차와 핵심 내용을 구성해줘. 총 10장 내외로 스토리텔링이 이어지도록 짜줘.</t>
-  </si>
-  <si>
-    <t>트위터 스레드 생성기</t>
-  </si>
-  <si>
-    <t>트위터(X)에서 많은 리트윗을 받을 수 있는 정보성 스레드(Thread)를 작성해줘. 첫 트윗은 호기심을 자극하고, 이어지는 트윗들은 유용한 정보를 간결하게 전달해줘.</t>
-  </si>
-  <si>
-    <t>엑셀 수식 설명기</t>
-  </si>
-  <si>
-    <t>복잡한 엑셀 함수나 수식이 어떻게 작동하는지 초등학생도 이해할 수 있게 쉽게 설명해줘. 실제 예시 데이터를 들어서 단계별로 풀이해줘.</t>
-  </si>
-  <si>
-    <t>소설 캐릭터 배경 설정</t>
-  </si>
-  <si>
-    <t>소설에 등장할 입체적인 캐릭터의 배경 스토리(Backstory)를 창작해줘. 성격, 외모, 트라우마, 목표, 특징적인 습관 등을 상세하게 묘사해줘.</t>
-  </si>
-  <si>
-    <t>상품 상세페이지 개선</t>
-  </si>
-  <si>
-    <t>쇼핑몰 상품 상세페이지의 구매 전환율을 높일 수 있도록 제품 설명 문구를 매력적으로 개선해줘. 고객의 니즈를 건드리고 제품의 장점을 감성적으로 어필해줘.</t>
+    <t>B2B 링크드인 리드 생성 전략</t>
+  </si>
+  <si>
+    <t>링크드인(LinkedIn)을 통해 잠재 고객(Lead)을 발굴하는 B2B 마케팅 전략을 작성해줘. 프로필 최적화 방법, 진정성 있는 네트워킹 메시지 예시, 그리고 ‘생각 리더(Thought Leader)’로 포지셔닝하기 위한 콘텐츠 주제 3가지를 포함해줘.</t>
+  </si>
+  <si>
+    <t>Next.js 14 서버 액션 실전 가이드</t>
+  </si>
+  <si>
+    <t>프론트엔드 개발자를 위해 Next.js 14의 'Server Actions' 기능을 완벽하게 해설해줘. 기존 API 라우트와의 차이점을 설명하고, 폼(Form) 데이터를 처리하는 안전한 코드 스니펫과 에러 핸들링 방법을 단계별로 작성해줘.</t>
+  </si>
+  <si>
+    <t>SaaS 이탈률(Churn Rate) 개선법</t>
+  </si>
+  <si>
+    <t>구독형 소프트웨어(SaaS) 비즈니스에서 고객 이탈률을 획기적으로 줄이는 5가지 전략을 상세히 기술해줘. 코호트 분석(Cohort Analysis)의 중요성을 언급하고, 이탈 방지를 위한 고객 성공(CS) 팀의 체크리스트를 만들어줘.</t>
+  </si>
+  <si>
+    <t>노션(Notion) '세컨드 브레인' 템플릿 설계</t>
+  </si>
+  <si>
+    <t>생산성을 극대화하는 노션 대시보드 구조를 제안해줘. PARA 방법론(Projects, Areas, Resources, Archives)에 기반하여 데이터베이스를 어떻게 연결해야 하는지 설명하고, 초보자도 따라 할 수 있는 세팅 순서를 알려줘.</t>
+  </si>
+  <si>
+    <t>생산성</t>
+  </si>
+  <si>
+    <t>스테이블 디퓨전 LoRA 학습 가이드</t>
+  </si>
+  <si>
+    <t>AI 이미지 생성 툴인 스테이블 디퓨전(Stable Diffusion)에서 나만의 LoRA 모델을 학습시키는 방법을 기술적인 가이드로 작성해줘. 학습용 이미지 전처리 방법, 캡셔닝 요령, 그리고 최적의 학습 파라미터 설정을 다뤄줘.</t>
+  </si>
+  <si>
+    <t>AI아트</t>
+  </si>
+  <si>
+    <t>판타지 소설 경제 시스템 구축법</t>
+  </si>
+  <si>
+    <t>판타지 소설 작가를 위해 현실감 있는 '가상 화폐 및 경제 시스템'을 만드는 법을 알려줘. 마법이 경제에 미치는 영향, 물가 상승 요인, 무역 루트 설정 등 세계관의 깊이를 더해주는 요소를 구체적으로 묘사해줘.</t>
+  </si>
+  <si>
+    <t>원격 근무 팀 갈등 해결 매뉴얼</t>
+  </si>
+  <si>
+    <t>100% 리모트 워크 환경에서 발생하는 팀원 간의 소통 오해와 갈등을 해결하는 리더십 가이드를 작성해줘. 텍스트 커뮤니케이션의 뉘앙스 파악법과 비대면 1:1 면담 시 사용할 수 있는 공감 대화 스크립트를 포함해줘.</t>
+  </si>
+  <si>
+    <t>리더십</t>
+  </si>
+  <si>
+    <t>뉴스레터 오픈율 30% 달성 제목 공식</t>
+  </si>
+  <si>
+    <t>구독자가 무조건 클릭하게 만드는 뉴스레터 제목 패턴 10가지를 정리해줘. 심리학적 트리거(호기심, 긴급성, 이득)를 활용한 예시와 함께, 미리보기 텍스트(Preheader)를 활용해 오픈율을 높이는 팁을 추가해줘.</t>
+  </si>
+  <si>
+    <t>도커(Docker) 이미지 경량화 노하우</t>
+  </si>
+  <si>
+    <t>데브옵스 엔지니어를 위해 도커 이미지 용량을 90%까지 줄이는 최적화 기법을 설명해줘. 멀티 스테이지 빌드(Multi-stage build)와 알파인 리눅스 활용법을 코드 예시(Dockerfile)와 함께 비교 분석해줘.</t>
+  </si>
+  <si>
+    <t>데브옵스</t>
+  </si>
+  <si>
+    <t>N잡러를 위한 종합소득세 절세 치트키</t>
+  </si>
+  <si>
+    <t>부업을 하는 직장인이나 프리랜서를 위한 종합소득세 신고 가이드를 작성해줘. 경비 처리 가능한 항목(식대, 장비 등)을 구체적으로 나열하고, 간편장부와 복식부기의 차이를 알기 쉽게 설명해줘.</t>
+  </si>
+  <si>
+    <t>재테크</t>
+  </si>
+  <si>
+    <t>스마트스토어 상세페이지 심리전</t>
+  </si>
+  <si>
+    <t>고객의 구매 심리를 자극하는 상세페이지 기획 구성을 5단계(문제 인식-공감-해결책-증거-행동 촉구)로 나누어 설명해줘. 각 단계별로 반드시 들어가야 할 문구 예시와 GIF 활용 팁을 작성해줘.</t>
+  </si>
+  <si>
+    <t>이커머스</t>
+  </si>
+  <si>
+    <t>파이썬기반 주식 자동매매 알고리즘</t>
+  </si>
+  <si>
+    <t>파이썬 라이브러리(ccxt 또는 pyupbit)를 활용해 이동평균선 골든크로스 전략을 사용하는 자동매매 봇의 기본 구조를 짜줘. 백테스팅(Backtesting)의 중요성과 리스크 관리(손절매) 코드를 반드시 포함해줘.</t>
+  </si>
+  <si>
+    <t>유튜브 숏츠 수익화 채널 기획</t>
+  </si>
+  <si>
+    <t>얼굴을 공개하지 않고(Faceless) 운영할 수 있는 고수익 유튜브 숏츠 채널 아이디어 5가지를 제안해줘. 각 아이디어별 소스 영상 구하는 법, AI 보이스 활용법, 추천 편집 툴을 패키지로 묶어서 소개해줘.</t>
+  </si>
+  <si>
+    <t>부업</t>
+  </si>
+  <si>
+    <t>UX 라이팅: 마이크로 카피 작성법</t>
+  </si>
+  <si>
+    <t>앱 사용자의 이탈을 막고 행동을 유도하는 버튼, 에러 메시지, 로딩 문구 등 '마이크로 카피' 작성 원칙을 알려줘. 딱딱한 개발자 용어를 사용자 친화적인 언어로 바꾼 Before &amp; After 예시를 5개 보여줘.</t>
+  </si>
+  <si>
+    <t>디자인</t>
+  </si>
+  <si>
+    <t>장/단기 기억 활용 학습법(Anki)</t>
+  </si>
+  <si>
+    <t>뇌과학에 기반한 효율적인 공부법과 간격 반복 시스템(SRS) 툴인 'Anki' 활용법을 작성해줘. 망각 곡선 이론을 설명하고, 암기 카드를 효율적으로 만드는 구조화(Cloze deletion 등) 팁을 공유해줘.</t>
+  </si>
+  <si>
+    <t>자기계발</t>
   </si>
 </sst>
 </file>
@@ -220,21 +217,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
@@ -249,19 +231,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -568,245 +569,223 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35.125" customWidth="1"/>
+    <col min="2" max="2" width="83.25" customWidth="1"/>
+    <col min="3" max="3" width="23.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="257.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:3" ht="370.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="327.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="342" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="356.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="342" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="313.5" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="243" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="271.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="257.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="257.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="257.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="285.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:3" ht="327.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="285.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
+      <c r="B9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="257.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+    </row>
+    <row r="10" spans="1:3" ht="327.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C10" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="327.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="228.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="B11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="243" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="285" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="200.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="C12" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="3" t="s">
+    </row>
+    <row r="13" spans="1:3" ht="299.25" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="257.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+      <c r="B13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="C13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="228.75" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+    </row>
+    <row r="14" spans="1:3" ht="313.5" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="243" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="C14" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="327.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="257.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3" t="s">
+      <c r="C15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="3" t="s">
+    </row>
+    <row r="16" spans="1:3" ht="299.25" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="200.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="B16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C16" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="214.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
+    </row>
+    <row r="17" spans="1:3" ht="299.25" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="243" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="C17" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>5</v>
-      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>